<commit_message>
Rédaction de la documentation
Finition de l'interface graphique et rédactiond de la documentation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
   <si>
     <t>DATE</t>
   </si>
@@ -294,6 +294,12 @@
   </si>
   <si>
     <t>Amelioration de l'interface graphique de la generation de terrain</t>
+  </si>
+  <si>
+    <t>45 min</t>
+  </si>
+  <si>
+    <t>Amélioration + finitions de l'interface graphique de la génération de terrain</t>
   </si>
 </sst>
 </file>
@@ -607,8 +613,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E41" totalsRowShown="0">
-  <autoFilter ref="B2:E41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E42" totalsRowShown="0">
+  <autoFilter ref="B2:E42"/>
   <tableColumns count="4">
     <tableColumn id="1" name="DATE" dataCellStyle="Date Column"/>
     <tableColumn id="2" name="HEURE" dataCellStyle="Time Column"/>
@@ -855,10 +861,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E41"/>
+  <dimension ref="B1:E42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1101,21 +1107,29 @@
       <c r="B19" s="11">
         <v>43147</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>91</v>
+      </c>
       <c r="E19" s="10"/>
     </row>
     <row r="20" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="11">
-        <v>43157</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="3">
+        <v>43147</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>87</v>
+      </c>
       <c r="E20" s="10"/>
     </row>
     <row r="21" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
-        <v>43158</v>
+        <v>43157</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4"/>
@@ -1123,7 +1137,7 @@
     </row>
     <row r="22" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
-        <v>371878</v>
+        <v>43158</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4"/>
@@ -1131,7 +1145,7 @@
     </row>
     <row r="23" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
-        <v>43161</v>
+        <v>371878</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4"/>
@@ -1139,7 +1153,7 @@
     </row>
     <row r="24" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
-        <v>43164</v>
+        <v>43161</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="4"/>
@@ -1147,7 +1161,7 @@
     </row>
     <row r="25" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
-        <v>43165</v>
+        <v>43164</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="4"/>
@@ -1155,7 +1169,7 @@
     </row>
     <row r="26" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="4"/>
@@ -1163,7 +1177,7 @@
     </row>
     <row r="27" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
-        <v>43168</v>
+        <v>43167</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="4"/>
@@ -1171,7 +1185,7 @@
     </row>
     <row r="28" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
-        <v>43171</v>
+        <v>43168</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4"/>
@@ -1179,7 +1193,7 @@
     </row>
     <row r="29" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
-        <v>43172</v>
+        <v>43171</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="4"/>
@@ -1187,7 +1201,7 @@
     </row>
     <row r="30" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
-        <v>43174</v>
+        <v>43172</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="4"/>
@@ -1195,7 +1209,7 @@
     </row>
     <row r="31" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>43175</v>
+        <v>43174</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="4"/>
@@ -1203,7 +1217,7 @@
     </row>
     <row r="32" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>43178</v>
+        <v>43175</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="4"/>
@@ -1211,7 +1225,7 @@
     </row>
     <row r="33" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>43179</v>
+        <v>43178</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="4"/>
@@ -1219,7 +1233,7 @@
     </row>
     <row r="34" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>43181</v>
+        <v>43179</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="4"/>
@@ -1227,7 +1241,7 @@
     </row>
     <row r="35" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>43185</v>
+        <v>43181</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="4"/>
@@ -1235,7 +1249,7 @@
     </row>
     <row r="36" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>43186</v>
+        <v>43185</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="4"/>
@@ -1243,7 +1257,7 @@
     </row>
     <row r="37" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
-        <v>43188</v>
+        <v>43186</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="4"/>
@@ -1251,7 +1265,7 @@
     </row>
     <row r="38" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
-        <v>43206</v>
+        <v>43188</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="4"/>
@@ -1259,7 +1273,7 @@
     </row>
     <row r="39" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
-        <v>43207</v>
+        <v>43206</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="4"/>
@@ -1267,7 +1281,7 @@
     </row>
     <row r="40" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
-        <v>43209</v>
+        <v>43207</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="4"/>
@@ -1275,11 +1289,19 @@
     </row>
     <row r="41" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
-        <v>43210</v>
+        <v>43209</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="4"/>
       <c r="E41" s="10"/>
+    </row>
+    <row r="42" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <v>43210</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="10"/>
     </row>
   </sheetData>
   <dataValidations xWindow="45" yWindow="267" count="5">
@@ -1606,6 +1628,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1786,27 +1828,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1823,22 +1863,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Code manadgement and Unity Hierarchy cleaning
Cleaned up the code, added comments and changed unity hierarchy script appending
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
   <si>
     <t>DATE</t>
   </si>
@@ -321,6 +321,12 @@
   </si>
   <si>
     <t>Recherche sur la génération de texture et liaison de l'interface graphiques aux données de la texture</t>
+  </si>
+  <si>
+    <t>Entretient du code et de la hierarchie de Unity</t>
+  </si>
+  <si>
+    <t>Ajout d'un fichier executable</t>
   </si>
 </sst>
 </file>
@@ -334,7 +340,7 @@
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="3" tint="9.982604449598681E-2"/>
@@ -418,6 +424,14 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -492,7 +506,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -519,8 +533,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -560,10 +577,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="12" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Date Column" xfId="3"/>
     <cellStyle name="Event Column" xfId="4"/>
+    <cellStyle name="Lien hypertexte" xfId="12" builtinId="8"/>
     <cellStyle name="Milliers" xfId="5" builtinId="3" customBuiltin="1"/>
     <cellStyle name="Milliers [0]" xfId="6" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Monétaire" xfId="7" builtinId="4" customBuiltin="1"/>
@@ -634,8 +655,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E44" totalsRowShown="0">
-  <autoFilter ref="B2:E44"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E45" totalsRowShown="0">
+  <autoFilter ref="B2:E45"/>
   <tableColumns count="4">
     <tableColumn id="1" name="DATE" dataCellStyle="Date Column"/>
     <tableColumn id="2" name="HEURE" dataCellStyle="Time Column"/>
@@ -882,10 +903,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E44"/>
+  <dimension ref="B1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1208,21 +1229,27 @@
       <c r="D25" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="11">
-        <v>43161</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="10"/>
+      <c r="B26" s="3">
+        <v>43160</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="27" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
-        <v>43164</v>
+        <v>43161</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="4"/>
@@ -1230,7 +1257,7 @@
     </row>
     <row r="28" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
-        <v>43165</v>
+        <v>43164</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4"/>
@@ -1238,7 +1265,7 @@
     </row>
     <row r="29" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="4"/>
@@ -1246,7 +1273,7 @@
     </row>
     <row r="30" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
-        <v>43168</v>
+        <v>43167</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="4"/>
@@ -1254,7 +1281,7 @@
     </row>
     <row r="31" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>43171</v>
+        <v>43168</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="4"/>
@@ -1262,7 +1289,7 @@
     </row>
     <row r="32" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>43172</v>
+        <v>43171</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="4"/>
@@ -1270,7 +1297,7 @@
     </row>
     <row r="33" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>43174</v>
+        <v>43172</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="4"/>
@@ -1278,7 +1305,7 @@
     </row>
     <row r="34" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>43175</v>
+        <v>43174</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="4"/>
@@ -1286,7 +1313,7 @@
     </row>
     <row r="35" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>43178</v>
+        <v>43175</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="4"/>
@@ -1294,7 +1321,7 @@
     </row>
     <row r="36" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>43179</v>
+        <v>43178</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="4"/>
@@ -1302,7 +1329,7 @@
     </row>
     <row r="37" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
-        <v>43181</v>
+        <v>43179</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="4"/>
@@ -1310,7 +1337,7 @@
     </row>
     <row r="38" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11">
-        <v>43185</v>
+        <v>43181</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="4"/>
@@ -1318,7 +1345,7 @@
     </row>
     <row r="39" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11">
-        <v>43186</v>
+        <v>43185</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="4"/>
@@ -1326,7 +1353,7 @@
     </row>
     <row r="40" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
-        <v>43188</v>
+        <v>43186</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="4"/>
@@ -1334,7 +1361,7 @@
     </row>
     <row r="41" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
-        <v>43206</v>
+        <v>43188</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="4"/>
@@ -1342,7 +1369,7 @@
     </row>
     <row r="42" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
-        <v>43207</v>
+        <v>43206</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="4"/>
@@ -1350,7 +1377,7 @@
     </row>
     <row r="43" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11">
-        <v>43209</v>
+        <v>43207</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="4"/>
@@ -1358,11 +1385,19 @@
     </row>
     <row r="44" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
-        <v>43210</v>
+        <v>43209</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="4"/>
       <c r="E44" s="10"/>
+    </row>
+    <row r="45" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="11">
+        <v>43210</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="10"/>
     </row>
   </sheetData>
   <dataValidations xWindow="45" yWindow="267" count="5">
@@ -1372,14 +1407,17 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Assurez le suivi des événements en fonction de la date, de l’heure et de la description de l’événement dans cet agenda. Entrer les informations dans la tableau Journal." sqref="A1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Le titre de l’agenda se trouve dans les cellules B1 à C1" sqref="B1"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E25" r:id="rId1"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId2"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1689,6 +1727,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1869,27 +1927,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1906,22 +1962,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rules for Procedural texturing
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="102">
   <si>
     <t>DATE</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Ajout d'un fichier executable</t>
+  </si>
+  <si>
+    <t>Recherche et expérimentation sur les règles a instaurer pour génerer des textures</t>
   </si>
 </sst>
 </file>
@@ -905,8 +908,8 @@
   </sheetPr>
   <dimension ref="B1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1251,8 +1254,12 @@
       <c r="B27" s="11">
         <v>43161</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="4"/>
+      <c r="C27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>101</v>
+      </c>
       <c r="E27" s="10"/>
     </row>
     <row r="28" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,26 +1734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1927,25 +1914,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1962,4 +1951,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
15.3.2018 HeightMap Texture Generation
Generates on texture only for now on, added lake/water generation
</commit_message>
<xml_diff>
--- a/Documentation/Journal de travail.xlsx
+++ b/Documentation/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="122">
   <si>
     <t>DATE</t>
   </si>
@@ -342,6 +342,54 @@
   </si>
   <si>
     <t>315 min</t>
+  </si>
+  <si>
+    <t>Recherche sur le placement des arbres</t>
+  </si>
+  <si>
+    <t>Recherche sur la génération de l'environnement aquatique</t>
+  </si>
+  <si>
+    <t>Après refflexion générer un environnement aquatique avant les autres arbres semble plus logique</t>
+  </si>
+  <si>
+    <t>Devellopement des rivières</t>
+  </si>
+  <si>
+    <t>génère des points aléatoires en auteur sur le heighmap</t>
+  </si>
+  <si>
+    <t>Reflexion sur papier sur comment trouver le points le plus proche et bas pour la rivière</t>
+  </si>
+  <si>
+    <t>travail a la maison</t>
+  </si>
+  <si>
+    <t>120 min</t>
+  </si>
+  <si>
+    <t>tentative d'implémentation de l'algorythme</t>
+  </si>
+  <si>
+    <t>recherches sur des algorythmes de pathfinder</t>
+  </si>
+  <si>
+    <t>travail a la maison, pour l'instant les rivières sont un trait droit, il faut que la rivière suive un chemin logique jusque a son point de destination</t>
+  </si>
+  <si>
+    <t>reflexion sur papier pour ameliorer l'algorythme de generation de rivieres</t>
+  </si>
+  <si>
+    <t>195 min</t>
+  </si>
+  <si>
+    <t>changement de l'approche sur l'interface graphique</t>
+  </si>
+  <si>
+    <t>desormer on vois plus que le heighmap avec les changements qui se font le terrain se génèrera a la fin</t>
+  </si>
+  <si>
+    <t>Generation des lacs/Ocean sur le heightMap</t>
   </si>
 </sst>
 </file>
@@ -670,8 +718,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E45" totalsRowShown="0">
-  <autoFilter ref="B2:E45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E50" totalsRowShown="0">
+  <autoFilter ref="B2:E50"/>
   <tableColumns count="4">
     <tableColumn id="1" name="DATE" dataCellStyle="Date Column"/>
     <tableColumn id="2" name="HEURE" dataCellStyle="Time Column"/>
@@ -918,10 +966,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E45"/>
+  <dimension ref="B1:E50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1311,77 +1359,125 @@
       <c r="B31" s="11">
         <v>43168</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="4"/>
+      <c r="C31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>106</v>
+      </c>
       <c r="E31" s="10"/>
     </row>
     <row r="32" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
         <v>43171</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="10"/>
+      <c r="C32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="33" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
         <v>43172</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="10"/>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="34" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11">
-        <v>43174</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="10"/>
+      <c r="B34" s="3">
+        <v>43172</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="35" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11">
-        <v>43175</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="10"/>
+      <c r="B35" s="3">
+        <v>43173</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="36" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11">
-        <v>43178</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="10"/>
+      <c r="B36" s="3">
+        <v>43173</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="37" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11">
-        <v>43179</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="4"/>
+        <v>43174</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>117</v>
+      </c>
       <c r="E37" s="10"/>
     </row>
     <row r="38" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11">
-        <v>43181</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="10"/>
+      <c r="B38" s="3">
+        <v>43174</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="39" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11">
-        <v>43185</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="4"/>
+      <c r="B39" s="3">
+        <v>43174</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>121</v>
+      </c>
       <c r="E39" s="10"/>
     </row>
     <row r="40" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11">
-        <v>43186</v>
+        <v>43175</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="4"/>
@@ -1389,7 +1485,7 @@
     </row>
     <row r="41" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11">
-        <v>43188</v>
+        <v>43178</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="4"/>
@@ -1397,7 +1493,7 @@
     </row>
     <row r="42" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11">
-        <v>43206</v>
+        <v>43179</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="4"/>
@@ -1405,7 +1501,7 @@
     </row>
     <row r="43" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11">
-        <v>43207</v>
+        <v>43181</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="4"/>
@@ -1413,7 +1509,7 @@
     </row>
     <row r="44" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="11">
-        <v>43209</v>
+        <v>43185</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="4"/>
@@ -1421,11 +1517,51 @@
     </row>
     <row r="45" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="11">
-        <v>43210</v>
+        <v>43186</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="4"/>
       <c r="E45" s="10"/>
+    </row>
+    <row r="46" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="11">
+        <v>43188</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="11">
+        <v>43206</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="11">
+        <v>43207</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="11">
+        <v>43209</v>
+      </c>
+      <c r="C49" s="2"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="11">
+        <v>43210</v>
+      </c>
+      <c r="C50" s="2"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="10"/>
     </row>
   </sheetData>
   <dataValidations xWindow="45" yWindow="267" count="5">
@@ -1756,6 +1892,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1936,27 +2092,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1973,22 +2127,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>